<commit_message>
Added Ganeshs version of Translate GL Account
</commit_message>
<xml_diff>
--- a/excel-data-files/currrency-transfer-ledger-balances.xlsx
+++ b/excel-data-files/currrency-transfer-ledger-balances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardguy/r/oracleplaywright/excel-data-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C58EB6-6811-C048-87B2-6CF6047F2E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1235ABF-9F74-6146-9F19-9FC61885BFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17860" yWindow="760" windowWidth="16700" windowHeight="21580" activeTab="2" xr2:uid="{39C55B49-5ADB-CF4F-8459-6E15E59B12DD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
   <si>
     <t>url</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Jan-18</t>
+  </si>
+  <si>
+    <t>Feb-18</t>
   </si>
 </sst>
 </file>
@@ -742,9 +745,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA25780A-EA5B-9148-8FFA-6154678F87EB}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -773,6 +778,17 @@
       </c>
       <c r="C2" s="6" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial update to ExcelService to allow overwriting results in same file
</commit_message>
<xml_diff>
--- a/excel-data-files/currrency-transfer-ledger-balances.xlsx
+++ b/excel-data-files/currrency-transfer-ledger-balances.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardguy/r/oracleplaywright/excel-data-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38960293-86B2-D94B-8E22-42D0E9D6A119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E3B0C0-8DA6-CC49-860D-651704A6D083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="760" windowWidth="16680" windowHeight="21580" xr2:uid="{39C55B49-5ADB-CF4F-8459-6E15E59B12DD}"/>
+    <workbookView xWindow="5640" yWindow="3180" windowWidth="25780" windowHeight="18760" firstSheet="2" activeTab="2" xr2:uid="{39C55B49-5ADB-CF4F-8459-6E15E59B12DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
     <sheet name="Setup" sheetId="1" r:id="rId2"/>
-    <sheet name="Loop" sheetId="6" r:id="rId3"/>
+    <sheet name="Loop" sheetId="11" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Loop!$A$1:$D$1211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Loop!$A$1:$V$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,44 +41,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+  <si>
+    <t>Instructions:</t>
+  </si>
+  <si>
+    <t>This data file must have the same filename as the Playwright test script, and must be stored in the excel-data-files folder.</t>
+  </si>
+  <si>
+    <t>Use the Setup sheet (Column B) for the values required only once. (Titles in column A can be whatever you like).</t>
+  </si>
+  <si>
+    <t>Use the Loop sheet (Rows 2 onwards) for values required many times. (Titles on Row 1 can be whatever you like).</t>
+  </si>
+  <si>
+    <t>Any other format will not work!</t>
+  </si>
   <si>
     <t>url</t>
   </si>
   <si>
+    <t>https://iahdme-dev1.fa.ocs.oraclecloud.com/</t>
+  </si>
+  <si>
     <t>newProcessName</t>
   </si>
   <si>
-    <t>Use the Loop sheet (Rows 2 onwards) for values required many times. (Titles on Row 1 can be whatever you like).</t>
-  </si>
-  <si>
-    <t>Instructions:</t>
-  </si>
-  <si>
-    <t>Use the Setup sheet (Column B) for the values required only once. (Titles in column A can be whatever you like).</t>
-  </si>
-  <si>
-    <t>Any other format will not work!</t>
-  </si>
-  <si>
-    <t>This data file must have the same filename as the Playwright test script, and must be stored in the excel-data-files folder.</t>
-  </si>
-  <si>
     <t>Transfer Ledger Balances</t>
   </si>
   <si>
     <t>Source Ledger</t>
   </si>
   <si>
+    <t>N/A - See Loop Worksheet!</t>
+  </si>
+  <si>
     <t>Target Ledger</t>
   </si>
   <si>
     <t>CoA Mapping</t>
   </si>
   <si>
+    <t>XX Secondary Ledger Balance</t>
+  </si>
+  <si>
     <t>Amount Type</t>
   </si>
   <si>
+    <t>PTD Period to date balance type.</t>
+  </si>
+  <si>
     <t>Run Journal Import</t>
   </si>
   <si>
@@ -88,28 +100,40 @@
     <t>Run Automatic Posting</t>
   </si>
   <si>
-    <t>N/A - See Loop Worksheet!</t>
-  </si>
-  <si>
-    <t>XX Secondary Ledger Balance</t>
-  </si>
-  <si>
-    <t>PTD Period to date balance type.</t>
-  </si>
-  <si>
-    <t>https://iahdme-test.fa.ocs.oraclecloud.com/fscmUI/faces/FuseOverview</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jul-21 </t>
-  </si>
-  <si>
-    <t>UK ACTUALS GBP Dec</t>
-  </si>
-  <si>
-    <t>UK ACTUALS GBP April</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apr-22 </t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Target ledger</t>
+  </si>
+  <si>
+    <t>Source Ledger Period</t>
+  </si>
+  <si>
+    <t>Target Ledger Period</t>
+  </si>
+  <si>
+    <t>Target Period</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>PERIOD_NAME</t>
+  </si>
+  <si>
+    <t>REQUESTID</t>
+  </si>
+  <si>
+    <t>STARTTIME</t>
+  </si>
+  <si>
+    <t>ENDTIME</t>
+  </si>
+  <si>
+    <t>RESULT</t>
   </si>
   <si>
     <t>IT ACTUALS EUR Apr</t>
@@ -118,58 +142,62 @@
     <t>IT ACTUALS EUR April</t>
   </si>
   <si>
-    <t xml:space="preserve">01_May-19 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oct-19 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">14_Apr-21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec-21 </t>
-  </si>
-  <si>
-    <t>Target ledger</t>
-  </si>
-  <si>
-    <t>Source Ledger Period</t>
-  </si>
-  <si>
-    <t>Target Ledger Period</t>
-  </si>
-  <si>
-    <t>Dec-21</t>
-  </si>
-  <si>
-    <t>Apr-22</t>
-  </si>
-  <si>
-    <t>May-19</t>
-  </si>
-  <si>
-    <t>Oct-19</t>
-  </si>
-  <si>
-    <t>Apr-21</t>
+    <t>Aug-18</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>Dec-18</t>
+  </si>
+  <si>
+    <t>STARTED</t>
+  </si>
+  <si>
+    <t>May-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01_May-21 </t>
+  </si>
+  <si>
+    <t>May-21</t>
+  </si>
+  <si>
+    <t>Mar-23</t>
+  </si>
+  <si>
+    <t>Jan-24</t>
+  </si>
+  <si>
+    <t>Dec-24</t>
+  </si>
+  <si>
+    <t>UY ACTUALS UYU Mar</t>
+  </si>
+  <si>
+    <t>UY ACTUALS UYU April</t>
+  </si>
+  <si>
+    <t>Nov-23</t>
+  </si>
+  <si>
+    <t>CL ACTUALS CLP Dec</t>
+  </si>
+  <si>
+    <t>CL ACTUALS CLP April</t>
+  </si>
+  <si>
+    <t>Jan-25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,6 +228,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -221,12 +270,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -247,25 +296,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF777777"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF777777"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF777777"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF777777"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,64 +682,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD33EC5-03CB-D544-9EAA-46900CFD2381}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="5.875" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="29.1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="29.1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="24.95" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="24.95" customHeight="1">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+    <row r="5" spans="1:2" ht="24.95" customHeight="1">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="7" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="8" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="9" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="10" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="11" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="12" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="13" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="14" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="15" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="16" spans="1:2" ht="24.95" customHeight="1"/>
+    <row r="17" ht="24.95" customHeight="1"/>
+    <row r="18" ht="24.95" customHeight="1"/>
+    <row r="19" ht="24.95" customHeight="1"/>
+    <row r="20" ht="24.95" customHeight="1"/>
+    <row r="21" ht="24.95" customHeight="1"/>
+    <row r="22" ht="24.95" customHeight="1"/>
+    <row r="23" ht="24.95" customHeight="1"/>
+    <row r="24" ht="24.95" customHeight="1"/>
+    <row r="25" ht="24.95" customHeight="1"/>
+    <row r="26" ht="24.95" customHeight="1"/>
+    <row r="27" ht="24.95" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -668,209 +750,657 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{14A53803-7D5F-FF41-AFDE-9D9DB84BDB7A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D626F8-F248-E240-85B0-ED4026E7A713}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FCD789-9BF8-CC4A-95BD-2C3C5B20BC77}">
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="24.875" hidden="1" customWidth="1"/>
+    <col min="9" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="11.875" hidden="1" customWidth="1"/>
+    <col min="16" max="18" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" s="12" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F11" si="0">B2&amp;TEXT(D2,"MMM-YY")</f>
+        <v>IT ACTUALS EUR AprAug-18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="e">
+        <f t="shared" ref="H2:H11" si="1">VLOOKUP(F2,P:P,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:R11" si="2">TEXT(D2,"MMM-YY")</f>
+        <v>Aug-18</v>
+      </c>
+      <c r="R2" t="str">
+        <f t="shared" si="2"/>
+        <v>Aug-18</v>
+      </c>
+      <c r="S2">
+        <v>23423</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>IT ACTUALS EUR AprDec-18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" si="2"/>
+        <v>Dec-18</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" si="2"/>
+        <v>Dec-18</v>
+      </c>
+      <c r="V3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>IT ACTUALS EUR AprMay-20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="2"/>
+        <v>May-20</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" si="2"/>
+        <v>May-20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">IT ACTUALS EUR Apr01_May-21 </v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">01_May-21 </v>
+      </c>
+      <c r="R5" t="str">
+        <f t="shared" si="2"/>
+        <v>May-21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>IT ACTUALS EUR AprMay-21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="2"/>
+        <v>May-21</v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="2"/>
+        <v>May-21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>IT ACTUALS EUR AprMar-23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="2"/>
+        <v>Mar-23</v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="2"/>
+        <v>Mar-23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>IT ACTUALS EUR AprJan-24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="2"/>
+        <v>Jan-24</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="2"/>
+        <v>Jan-24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>IT ACTUALS EUR AprDec-24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="2"/>
+        <v>Dec-24</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="2"/>
+        <v>Dec-24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>UY ACTUALS UYU MarNov-23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="2"/>
+        <v>Nov-23</v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" si="2"/>
+        <v>Nov-23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.95" customHeight="1">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>CL ACTUALS CLP DecJan-25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="2"/>
+        <v>Jan-25</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" si="2"/>
+        <v>Jan-25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.95" customHeight="1">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" ht="15.95" customHeight="1">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" ht="15.95" customHeight="1">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.95" customHeight="1">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" ht="15.95" customHeight="1">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="2:4" ht="15.95" customHeight="1">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="2:5" ht="15.95" customHeight="1">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1211" xr:uid="{0006A4B6-642B-944B-9FA8-B759DEAA9589}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>